<commit_message>
Auditoria y no conformidades
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1345 - AECCON, Guillermo Sandoval_MO/Calidad/No_conformidades.xlsx
+++ b/Proyectos/2015/11/P1345 - AECCON, Guillermo Sandoval_MO/Calidad/No_conformidades.xlsx
@@ -47,7 +47,7 @@
     <t>Oriana Osiris</t>
   </si>
   <si>
-    <t>En proceso</t>
+    <t>Cerrada</t>
   </si>
   <si>
     <t>Se requiere cambiar la versión del plan del proyecto ya que es una versión vieja, así como cambiar la redacción de riesgos en causa consecuencia, recursos materiales por los utilizados entre otros cambios como se muestran por ejemplo en plan de proyectos de p1366 por ejemplo</t>
@@ -306,8 +306,8 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>